<commit_message>
0528 crud element proc update
</commit_message>
<xml_diff>
--- a/중간발표/CRUD메트릭스.xlsx
+++ b/중간발표/CRUD메트릭스.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\데베설\git_corp\My-Cinema\중간발표\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7AB0488-B9FB-423B-9243-CA3F4AE66D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF44C07-F6C2-4C1A-BAFF-36885BD75EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23955" yWindow="2880" windowWidth="21210" windowHeight="15435" xr2:uid="{BF35880F-C2E3-41AF-9943-8008D55ED834}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{BF35880F-C2E3-41AF-9943-8008D55ED834}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="90">
   <si>
     <t>영화를 등록한다</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -389,6 +389,10 @@
   </si>
   <si>
     <t>고객정보를 삭제한다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>U, C</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -396,7 +400,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -420,8 +424,16 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -431,6 +443,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -443,23 +460,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="나쁨" xfId="2" builtinId="27"/>
     <cellStyle name="좋음" xfId="1" builtinId="26"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -773,10 +797,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7FCE492-328D-4B73-9660-E6C5C9C9FD95}">
-  <dimension ref="A1:AD47"/>
+  <dimension ref="A1:AE47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -791,15 +815,14 @@
     <col min="13" max="13" width="7.125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5.25" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.125" customWidth="1"/>
-    <col min="17" max="17" width="13" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="5.875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="5.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D1" t="s">
         <v>8</v>
       </c>
@@ -837,52 +860,52 @@
         <v>63</v>
       </c>
       <c r="P1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" t="s">
+        <v>80</v>
+      </c>
+      <c r="S1" t="s">
+        <v>64</v>
+      </c>
+      <c r="T1" t="s">
+        <v>52</v>
+      </c>
+      <c r="U1" t="s">
+        <v>53</v>
+      </c>
+      <c r="V1" t="s">
+        <v>54</v>
+      </c>
+      <c r="W1" t="s">
+        <v>55</v>
+      </c>
+      <c r="X1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>80</v>
-      </c>
-      <c r="T1" t="s">
-        <v>64</v>
-      </c>
-      <c r="U1" t="s">
-        <v>52</v>
-      </c>
-      <c r="V1" t="s">
-        <v>53</v>
-      </c>
-      <c r="W1" t="s">
-        <v>54</v>
-      </c>
-      <c r="X1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>79</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -896,7 +919,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
         <v>67</v>
       </c>
@@ -904,7 +927,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>84</v>
       </c>
@@ -918,7 +941,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
         <v>69</v>
       </c>
@@ -926,7 +949,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>85</v>
       </c>
@@ -943,7 +966,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C7" s="1" t="s">
         <v>71</v>
       </c>
@@ -951,7 +974,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>72</v>
       </c>
@@ -962,7 +985,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C9" s="1" t="s">
         <v>73</v>
       </c>
@@ -970,7 +993,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C10" s="1" t="s">
         <v>74</v>
       </c>
@@ -978,34 +1001,34 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>75</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AA11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="Z11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C12" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AA12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="Z12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C13" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AA13" t="s">
+      <c r="Z13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>33</v>
       </c>
@@ -1018,11 +1041,14 @@
       <c r="J14" t="s">
         <v>19</v>
       </c>
+      <c r="K14" t="s">
+        <v>19</v>
+      </c>
       <c r="L14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C15" s="1" t="s">
         <v>1</v>
       </c>
@@ -1035,11 +1061,14 @@
       <c r="J15" t="s">
         <v>21</v>
       </c>
+      <c r="K15" t="s">
+        <v>21</v>
+      </c>
       <c r="L15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>45</v>
       </c>
@@ -1053,7 +1082,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C17" s="1" t="s">
         <v>47</v>
       </c>
@@ -1061,7 +1090,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>34</v>
       </c>
@@ -1075,7 +1104,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C19" s="1" t="s">
         <v>3</v>
       </c>
@@ -1083,42 +1112,51 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>86</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="N20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="T21" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="S21" t="s">
+        <v>20</v>
+      </c>
+      <c r="X21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C22" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="Q22" t="s">
+        <v>20</v>
+      </c>
       <c r="R22" t="s">
         <v>20</v>
       </c>
-      <c r="S22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="C23" t="s">
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="C23" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="M23" t="s">
+        <v>21</v>
+      </c>
+      <c r="N23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -1134,11 +1172,11 @@
       <c r="N25" t="s">
         <v>19</v>
       </c>
-      <c r="Q25" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="P25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C26" s="1" t="s">
         <v>5</v>
       </c>
@@ -1146,7 +1184,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C27" s="1" t="s">
         <v>6</v>
       </c>
@@ -1156,33 +1194,33 @@
       <c r="N27" t="s">
         <v>21</v>
       </c>
-      <c r="Q27" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="P27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C28" s="1" t="s">
         <v>24</v>
       </c>
       <c r="N28" t="s">
         <v>20</v>
       </c>
-      <c r="Q28" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="P28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C29" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="Q29" t="s">
+        <v>20</v>
+      </c>
       <c r="R29" t="s">
         <v>20</v>
       </c>
-      <c r="S29" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>36</v>
       </c>
@@ -1195,11 +1233,14 @@
       <c r="J30" t="s">
         <v>20</v>
       </c>
+      <c r="K30" t="s">
+        <v>20</v>
+      </c>
       <c r="L30" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C31" s="1" t="s">
         <v>28</v>
       </c>
@@ -1209,14 +1250,17 @@
       <c r="J31" t="s">
         <v>20</v>
       </c>
+      <c r="K31" t="s">
+        <v>20</v>
+      </c>
       <c r="L31" t="s">
         <v>20</v>
       </c>
-      <c r="Q31" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="P31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C32" s="1" t="s">
         <v>39</v>
       </c>
@@ -1224,6 +1268,9 @@
         <v>20</v>
       </c>
       <c r="J32" t="s">
+        <v>20</v>
+      </c>
+      <c r="K32" t="s">
         <v>20</v>
       </c>
       <c r="L32" t="s">
@@ -1240,6 +1287,9 @@
       <c r="J33" t="s">
         <v>20</v>
       </c>
+      <c r="K33" t="s">
+        <v>20</v>
+      </c>
       <c r="L33" t="s">
         <v>20</v>
       </c>
@@ -1248,117 +1298,135 @@
       <c r="B34" t="s">
         <v>37</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" t="s">
+        <v>20</v>
+      </c>
+      <c r="E34" t="s">
+        <v>20</v>
+      </c>
+      <c r="F34" t="s">
+        <v>20</v>
+      </c>
+      <c r="H34" t="s">
+        <v>20</v>
+      </c>
+      <c r="I34" t="s">
+        <v>20</v>
+      </c>
+      <c r="K34" t="s">
+        <v>20</v>
+      </c>
+      <c r="M34" t="s">
+        <v>19</v>
+      </c>
+      <c r="O34" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="C35" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D35" t="s">
+        <v>20</v>
+      </c>
+      <c r="E35" t="s">
+        <v>20</v>
+      </c>
+      <c r="F35" t="s">
+        <v>20</v>
+      </c>
+      <c r="H35" t="s">
+        <v>20</v>
+      </c>
+      <c r="I35" t="s">
+        <v>20</v>
+      </c>
+      <c r="K35" t="s">
+        <v>20</v>
+      </c>
+      <c r="M35" t="s">
+        <v>19</v>
+      </c>
+      <c r="O35" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y35" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z35" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA35" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB35" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I34" t="s">
-        <v>20</v>
-      </c>
-      <c r="N34" t="s">
-        <v>20</v>
-      </c>
-      <c r="AB34" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="35" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="C35" t="s">
+      <c r="I36" t="s">
+        <v>20</v>
+      </c>
+      <c r="N36" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA36" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC36" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="C37" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I35" t="s">
-        <v>20</v>
-      </c>
-      <c r="O35" t="s">
-        <v>20</v>
-      </c>
-      <c r="AB35" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="36" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="C36" t="s">
-        <v>26</v>
-      </c>
-      <c r="D36" t="s">
-        <v>20</v>
-      </c>
-      <c r="E36" t="s">
-        <v>20</v>
-      </c>
-      <c r="F36" t="s">
-        <v>20</v>
-      </c>
-      <c r="H36" t="s">
-        <v>20</v>
-      </c>
-      <c r="I36" t="s">
-        <v>20</v>
-      </c>
-      <c r="M36" t="s">
-        <v>19</v>
-      </c>
-      <c r="O36" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z36" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA36" t="s">
-        <v>20</v>
-      </c>
-      <c r="AB36" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC36" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="C37" t="s">
-        <v>48</v>
-      </c>
-      <c r="D37" t="s">
-        <v>20</v>
-      </c>
-      <c r="E37" t="s">
-        <v>20</v>
-      </c>
-      <c r="F37" t="s">
-        <v>20</v>
-      </c>
-      <c r="H37" t="s">
-        <v>20</v>
-      </c>
       <c r="I37" t="s">
         <v>20</v>
       </c>
-      <c r="M37" t="s">
-        <v>19</v>
-      </c>
       <c r="O37" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z37" t="s">
         <v>20</v>
       </c>
       <c r="AA37" t="s">
-        <v>20</v>
-      </c>
-      <c r="AB37" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="AC37" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="38" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="C38" t="s">
+      <c r="C38" s="1" t="s">
         <v>30</v>
       </c>
       <c r="M38" t="s">
         <v>21</v>
       </c>
       <c r="O38" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA38" t="s">
         <v>21</v>
       </c>
       <c r="AB38" t="s">
@@ -1372,135 +1440,144 @@
       <c r="B39" t="s">
         <v>38</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="1" t="s">
         <v>56</v>
       </c>
+      <c r="S39" t="s">
+        <v>19</v>
+      </c>
       <c r="T39" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="U39" t="s">
-        <v>20</v>
-      </c>
-      <c r="V39" t="s">
-        <v>19</v>
-      </c>
-      <c r="AB39" t="s">
-        <v>20</v>
-      </c>
-      <c r="AC39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="40" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="C40" t="s">
+      <c r="C40" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="S40" t="s">
+        <v>19</v>
+      </c>
       <c r="T40" t="s">
-        <v>19</v>
-      </c>
-      <c r="U40" t="s">
-        <v>20</v>
-      </c>
-      <c r="W40" t="s">
+        <v>20</v>
+      </c>
+      <c r="V40" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="41" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="C41" t="s">
+      <c r="C41" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="S41" t="s">
+        <v>19</v>
+      </c>
       <c r="T41" t="s">
-        <v>19</v>
-      </c>
-      <c r="U41" t="s">
-        <v>20</v>
-      </c>
-      <c r="X41" t="s">
+        <v>20</v>
+      </c>
+      <c r="W41" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="42" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="C42" t="s">
+      <c r="C42" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N42" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>19</v>
+      </c>
+      <c r="R42" t="s">
+        <v>19</v>
+      </c>
+      <c r="S42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="C43" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L42" t="s">
+      <c r="L43" t="s">
         <v>22</v>
       </c>
-      <c r="M42" t="s">
-        <v>20</v>
-      </c>
-      <c r="T42" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y42" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="43" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="C43" t="s">
+      <c r="S43" t="s">
+        <v>20</v>
+      </c>
+      <c r="X43" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="C44" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="N43" t="s">
-        <v>22</v>
-      </c>
-      <c r="R43" t="s">
-        <v>19</v>
-      </c>
-      <c r="S43" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="44" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="C44" t="s">
-        <v>41</v>
       </c>
       <c r="N44" t="s">
         <v>22</v>
       </c>
+      <c r="Q44" t="s">
+        <v>19</v>
+      </c>
       <c r="R44" t="s">
         <v>19</v>
       </c>
-      <c r="S44" t="s">
-        <v>19</v>
-      </c>
-      <c r="T44" t="s">
-        <v>22</v>
+      <c r="X44" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="45" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="C45" t="s">
+      <c r="C45" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="M45" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y45" t="s">
+      <c r="S45" t="s">
+        <v>20</v>
+      </c>
+      <c r="X45" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="46" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="C46" t="s">
+      <c r="C46" s="1" t="s">
         <v>42</v>
       </c>
       <c r="L46" t="s">
         <v>22</v>
       </c>
-      <c r="M46" t="s">
-        <v>20</v>
+      <c r="Q46" t="s">
+        <v>19</v>
       </c>
       <c r="R46" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="S46" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y46" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+      <c r="X46" t="s">
+        <v>89</v>
+      </c>
+      <c r="AB46" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="47" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="C47" t="s">
+      <c r="C47" s="1" t="s">
         <v>59</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>20</v>
+      </c>
+      <c r="R47" t="s">
+        <v>20</v>
+      </c>
+      <c r="S47" t="s">
+        <v>20</v>
+      </c>
+      <c r="X47" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>